<commit_message>
Pivot tables and pivot charts
</commit_message>
<xml_diff>
--- a/Pivot tables & charts.xlsx
+++ b/Pivot tables & charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC98362-B362-49DC-BC15-06E101681A66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F41520-38DF-489E-A730-E249869E98D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{86BE1D2F-147F-404C-817D-CAF910123D7B}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="5" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -143,13 +143,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1506,7 +1511,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3C53ED3-EF8B-44F7-B45D-155CBB885C4F}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C3C53ED3-EF8B-44F7-B45D-155CBB885C4F}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="I3:O9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -1963,11 +1968,12 @@
   <dimension ref="B1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
@@ -1982,7 +1988,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" t="s">
@@ -1990,62 +1996,62 @@
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>23</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>250</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>300</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
@@ -2068,132 +2074,132 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>25</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>400</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>300</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
         <v>300</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>26</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <v>500</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
         <v>250</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>250</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
         <v>500</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>23</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
         <v>250</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2">
         <v>400</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3">
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
         <v>400</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2">
         <v>500</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="2">
         <v>500</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>300</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>250</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>250</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>400</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>500</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="2">
         <v>1700</v>
       </c>
     </row>

</xml_diff>